<commit_message>
layered architecture si entity framework (legatura cu baza de date)
</commit_message>
<xml_diff>
--- a/MatodeAvansate/Prezenta.xlsx
+++ b/MatodeAvansate/Prezenta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\MatodeAvansate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MatodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3240BFBA-88F4-4F75-B341-B2DFEAA0D7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EC7E14-7A29-48EE-828A-1B637AAF3D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -128,6 +128,21 @@
   </si>
   <si>
     <t>Petz Ervin</t>
+  </si>
+  <si>
+    <t>Paul Roxana</t>
+  </si>
+  <si>
+    <t>Olah Antonio</t>
+  </si>
+  <si>
+    <t>Bucsa Andrei</t>
+  </si>
+  <si>
+    <t>Dumitrache Luca</t>
+  </si>
+  <si>
+    <t>Sule Zsolt</t>
   </si>
 </sst>
 </file>
@@ -321,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -367,6 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -721,12 +737,12 @@
     </row>
     <row r="3" spans="2:19">
       <c r="B3" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -748,9 +764,10 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="5" t="b">
+        <v>39</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="P4" s="9"/>
@@ -763,11 +780,23 @@
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="18" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="11">
         <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
@@ -778,7 +807,7 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -793,67 +822,79 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="11">
         <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="11">
         <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="18" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="11">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="14"/>
       <c r="S9" s="15"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="11">
         <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="18" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -868,52 +909,61 @@
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="18" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="11">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="18" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="11">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="11">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -928,9 +978,10 @@
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="5" t="b">
+        <v>37</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
@@ -943,22 +994,25 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="11">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17" s="14"/>
       <c r="S17" s="15"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -973,9 +1027,10 @@
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="5" t="b">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
@@ -988,7 +1043,7 @@
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="18" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -1002,48 +1057,87 @@
       <c r="S20" s="15"/>
     </row>
     <row r="21" spans="2:19">
-      <c r="B21" s="18"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="11">
-        <f t="shared" ref="Q4:Q22" si="0">C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>0</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>2</v>
       </c>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
     </row>
     <row r="22" spans="2:19">
-      <c r="B22" s="18"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>2</v>
       </c>
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="18"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="9"/>
-      <c r="Q23" s="11"/>
+      <c r="Q23" s="11">
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>1</v>
+      </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
     <row r="24" spans="2:19">
-      <c r="B24" s="18"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="9"/>
-      <c r="Q24" s="11"/>
+      <c r="Q24" s="11">
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <v>2</v>
+      </c>
       <c r="R24" s="14"/>
       <c r="S24" s="15"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="18"/>
+      <c r="B25" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="C25" s="5"/>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="9"/>
-      <c r="Q25" s="11"/>
+      <c r="Q25" s="11">
+        <f t="shared" ref="Q22:Q27" si="0">C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>1</v>
+      </c>
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
     </row>
@@ -1051,7 +1145,10 @@
       <c r="B26" s="18"/>
       <c r="C26" s="5"/>
       <c r="P26" s="9"/>
-      <c r="Q26" s="11"/>
+      <c r="Q26" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
     </row>
@@ -1059,7 +1156,10 @@
       <c r="B27" s="18"/>
       <c r="C27" s="5"/>
       <c r="P27" s="9"/>
-      <c r="Q27" s="11"/>
+      <c r="Q27" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R27" s="14"/>
       <c r="S27" s="15"/>
     </row>
@@ -1223,8 +1323,8 @@
       <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S20">
-    <sortCondition ref="B3:B20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S24">
+    <sortCondition ref="B24"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q45">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 12.10.2023: Bazele la grafuri, citit din fisier, afisat, desenat graf
</commit_message>
<xml_diff>
--- a/MatodeAvansate/Prezenta.xlsx
+++ b/MatodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MatodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72BEAF8-7949-4CFA-8640-AE4C5CF6136D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19A36F-6CCD-4FC6-817E-A5D2288B892F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>Mondek Marka</t>
+  </si>
+  <si>
+    <t>Turani Narcis</t>
+  </si>
+  <si>
+    <t>Arva Andrei</t>
+  </si>
+  <si>
+    <t>Papp David</t>
+  </si>
+  <si>
+    <t>Oprea Dumitrel</t>
   </si>
 </sst>
 </file>
@@ -671,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -740,7 +752,7 @@
     </row>
     <row r="3" spans="2:19">
       <c r="B3" s="18" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="b">
@@ -767,12 +779,23 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
+      <c r="D4" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="11">
         <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
@@ -783,23 +806,12 @@
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
+        <v>39</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="11">
         <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
@@ -810,7 +822,7 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="18" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
@@ -825,25 +837,22 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="11">
         <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
@@ -861,7 +870,7 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C9" s="5" t="b">
         <v>1</v>
@@ -879,7 +888,7 @@
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -897,40 +906,40 @@
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="18" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="11">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="18" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="11">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -948,59 +957,61 @@
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="C14" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="11">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C15" s="5"/>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="11">
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R15" s="14"/>
       <c r="S15" s="15"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="11">
         <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" s="14"/>
       <c r="S16" s="15"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" t="b">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="9"/>
@@ -1013,40 +1024,41 @@
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="D18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="11">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="11">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="18" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" t="b">
@@ -1062,58 +1074,57 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="18" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C21" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="11">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="11">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C23" s="5"/>
       <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="11">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="18" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
@@ -1128,7 +1139,7 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -1146,52 +1157,84 @@
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="11">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
     </row>
     <row r="27" spans="2:19">
-      <c r="B27" s="18"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="11">
-        <f t="shared" ref="Q22:Q27" si="0">C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>0</v>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>1</v>
       </c>
       <c r="R27" s="14"/>
       <c r="S27" s="15"/>
     </row>
     <row r="28" spans="2:19">
-      <c r="B28" s="18"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="9"/>
-      <c r="Q28" s="11"/>
+      <c r="Q28" s="11">
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>2</v>
+      </c>
       <c r="R28" s="14"/>
       <c r="S28" s="15"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="B29" s="18"/>
+      <c r="B29" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="C29" s="5"/>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="9"/>
-      <c r="Q29" s="11"/>
+      <c r="Q29" s="11">
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>1</v>
+      </c>
       <c r="R29" s="14"/>
       <c r="S29" s="15"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="B30" s="18"/>
+      <c r="B30" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="C30" s="5"/>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="9"/>
-      <c r="Q30" s="11"/>
+      <c r="Q30" s="11">
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>1</v>
+      </c>
       <c r="R30" s="14"/>
       <c r="S30" s="15"/>
     </row>
@@ -1199,7 +1242,10 @@
       <c r="B31" s="18"/>
       <c r="C31" s="5"/>
       <c r="P31" s="9"/>
-      <c r="Q31" s="11"/>
+      <c r="Q31" s="11">
+        <f t="shared" ref="Q27:Q35" si="0">C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>0</v>
+      </c>
       <c r="R31" s="14"/>
       <c r="S31" s="15"/>
     </row>
@@ -1207,7 +1253,10 @@
       <c r="B32" s="18"/>
       <c r="C32" s="5"/>
       <c r="P32" s="9"/>
-      <c r="Q32" s="11"/>
+      <c r="Q32" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R32" s="14"/>
       <c r="S32" s="15"/>
     </row>
@@ -1215,7 +1264,10 @@
       <c r="B33" s="18"/>
       <c r="C33" s="5"/>
       <c r="P33" s="9"/>
-      <c r="Q33" s="11"/>
+      <c r="Q33" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R33" s="14"/>
       <c r="S33" s="15"/>
     </row>
@@ -1223,7 +1275,10 @@
       <c r="B34" s="18"/>
       <c r="C34" s="5"/>
       <c r="P34" s="9"/>
-      <c r="Q34" s="11"/>
+      <c r="Q34" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R34" s="14"/>
       <c r="S34" s="15"/>
     </row>
@@ -1231,7 +1286,10 @@
       <c r="B35" s="18"/>
       <c r="C35" s="5"/>
       <c r="P35" s="9"/>
-      <c r="Q35" s="11"/>
+      <c r="Q35" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R35" s="14"/>
       <c r="S35" s="15"/>
     </row>
@@ -1331,8 +1389,8 @@
       <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S26">
-    <sortCondition ref="B26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S30">
+    <sortCondition ref="B30"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q45">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
in memory database (in caz ca nu merge sql)
</commit_message>
<xml_diff>
--- a/MatodeAvansate/Prezenta.xlsx
+++ b/MatodeAvansate/Prezenta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MatodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19A36F-6CCD-4FC6-817E-A5D2288B892F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB38F66C-1DFC-40CE-A1D2-FC540B39D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>Oprea Dumitrel</t>
+  </si>
+  <si>
+    <t>Balog Serban</t>
+  </si>
+  <si>
+    <t>Cioara Luca</t>
+  </si>
+  <si>
+    <t>Stroescu Raul</t>
+  </si>
+  <si>
+    <t>Vancea Claudiu</t>
   </si>
 </sst>
 </file>
@@ -351,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,7 +409,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -779,23 +790,12 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="18" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="11">
         <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
@@ -806,25 +806,29 @@
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
         <v>1</v>
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="11">
         <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R5" s="14"/>
       <c r="S5" s="15"/>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="5" t="b">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="P6" s="9"/>
@@ -837,9 +841,10 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="5" t="b">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="P7" s="9"/>
@@ -852,12 +857,12 @@
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="18" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C8" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D8" t="b">
+      <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="P8" s="9"/>
@@ -870,25 +875,22 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="11">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R9" s="14"/>
       <c r="S9" s="15"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
@@ -906,112 +908,130 @@
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
       </c>
       <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="11">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="18" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="11">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="11">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="18" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="11">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C15" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
         <v>1</v>
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="11">
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R15" s="14"/>
       <c r="S15" s="15"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="18" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="11">
         <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R16" s="14"/>
       <c r="S16" s="15"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="5" t="b">
+        <v>41</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="9"/>
@@ -1024,41 +1044,43 @@
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="11">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="11">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="18" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" t="b">
@@ -1074,7 +1096,7 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -1092,7 +1114,7 @@
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" t="b">
@@ -1108,25 +1130,28 @@
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C23" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="11">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="5" t="b">
+        <v>44</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="9"/>
@@ -1139,79 +1164,82 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="11">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="18" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C26" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="11">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="11">
         <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R27" s="14"/>
       <c r="S27" s="15"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
       </c>
       <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="11">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R28" s="14"/>
       <c r="S28" s="15"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" t="b">
+        <v>25</v>
+      </c>
+      <c r="C29" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P29" s="9"/>
@@ -1224,60 +1252,85 @@
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C30" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D30" t="b">
         <v>1</v>
       </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="11">
         <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R30" s="14"/>
       <c r="S30" s="15"/>
     </row>
     <row r="31" spans="2:19">
-      <c r="B31" s="18"/>
+      <c r="B31" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="C31" s="5"/>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="11">
-        <f t="shared" ref="Q27:Q35" si="0">C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>0</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>1</v>
       </c>
       <c r="R31" s="14"/>
       <c r="S31" s="15"/>
     </row>
     <row r="32" spans="2:19">
-      <c r="B32" s="18"/>
+      <c r="B32" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="C32" s="5"/>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>2</v>
       </c>
       <c r="R32" s="14"/>
       <c r="S32" s="15"/>
     </row>
     <row r="33" spans="2:19">
-      <c r="B33" s="18"/>
+      <c r="B33" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="C33" s="5"/>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
       <c r="P33" s="9"/>
       <c r="Q33" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>1</v>
       </c>
       <c r="R33" s="14"/>
       <c r="S33" s="15"/>
     </row>
     <row r="34" spans="2:19">
-      <c r="B34" s="18"/>
+      <c r="B34" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="C34" s="5"/>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>1</v>
       </c>
       <c r="R34" s="14"/>
       <c r="S34" s="15"/>
@@ -1287,7 +1340,7 @@
       <c r="C35" s="5"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q31:Q39" si="0">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
         <v>0</v>
       </c>
       <c r="R35" s="14"/>
@@ -1297,7 +1350,10 @@
       <c r="B36" s="18"/>
       <c r="C36" s="5"/>
       <c r="P36" s="9"/>
-      <c r="Q36" s="11"/>
+      <c r="Q36" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R36" s="14"/>
       <c r="S36" s="15"/>
     </row>
@@ -1305,7 +1361,10 @@
       <c r="B37" s="18"/>
       <c r="C37" s="5"/>
       <c r="P37" s="9"/>
-      <c r="Q37" s="11"/>
+      <c r="Q37" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R37" s="14"/>
       <c r="S37" s="15"/>
     </row>
@@ -1313,7 +1372,10 @@
       <c r="B38" s="18"/>
       <c r="C38" s="5"/>
       <c r="P38" s="9"/>
-      <c r="Q38" s="11"/>
+      <c r="Q38" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R38" s="14"/>
       <c r="S38" s="15"/>
     </row>
@@ -1321,7 +1383,10 @@
       <c r="B39" s="18"/>
       <c r="C39" s="5"/>
       <c r="P39" s="9"/>
-      <c r="Q39" s="11"/>
+      <c r="Q39" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R39" s="14"/>
       <c r="S39" s="15"/>
     </row>
@@ -1389,8 +1454,8 @@
       <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S30">
-    <sortCondition ref="B30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S34">
+    <sortCondition ref="B34"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q45">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 19.10.2023 - colorearea hartii vizual
</commit_message>
<xml_diff>
--- a/MatodeAvansate/Prezenta.xlsx
+++ b/MatodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MatodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58956C2A-07B7-49FF-8353-63441D89293D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFD342A-4021-4A22-A22B-450AB2C45F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Mocan Bogdan</t>
+  </si>
+  <si>
+    <t>Rad Paul</t>
   </si>
 </sst>
 </file>
@@ -700,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -869,10 +872,13 @@
       <c r="D8" t="b">
         <v>1</v>
       </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="11">
         <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
@@ -1035,83 +1041,83 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C17" s="5"/>
       <c r="E17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="11">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R17" s="14"/>
       <c r="S17" s="15"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="11">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C19" s="5"/>
       <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="11">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="11">
         <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R20" s="14"/>
       <c r="S20" s="15"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" t="b">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="9"/>
@@ -1124,12 +1130,13 @@
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="9"/>
@@ -1142,28 +1149,34 @@
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="11">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C24" s="5"/>
       <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="9"/>
@@ -1176,23 +1189,28 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C25" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="11">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" t="b">
@@ -1208,9 +1226,10 @@
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="5" t="b">
+        <v>36</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="9"/>
@@ -1223,12 +1242,9 @@
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="18" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C28" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="b">
         <v>1</v>
       </c>
       <c r="E28" t="b">
@@ -1237,14 +1253,14 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="11">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R28" s="14"/>
       <c r="S28" s="15"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="5" t="b">
         <v>1</v>
@@ -1265,43 +1281,43 @@
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
         <v>1</v>
       </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="11">
         <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R30" s="14"/>
       <c r="S30" s="15"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="11">
         <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R31" s="14"/>
       <c r="S31" s="15"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="18" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C32" s="5"/>
       <c r="E32" t="b">
@@ -1317,9 +1333,11 @@
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C33" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
@@ -1329,17 +1347,17 @@
       <c r="P33" s="9"/>
       <c r="Q33" s="11">
         <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R33" s="14"/>
       <c r="S33" s="15"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="18" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" t="b">
+      <c r="E34" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="9"/>
@@ -1352,43 +1370,54 @@
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="18" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C35" s="5"/>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
       <c r="E35" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="11">
         <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R35" s="14"/>
       <c r="S35" s="15"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="18" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C36" s="5"/>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
       <c r="E36" t="b">
         <v>1</v>
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="11">
-        <f t="shared" ref="Q31:Q39" si="0">C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>1</v>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <v>2</v>
       </c>
       <c r="R36" s="14"/>
       <c r="S36" s="15"/>
     </row>
     <row r="37" spans="2:19">
-      <c r="B37" s="18"/>
+      <c r="B37" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="C37" s="5"/>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>1</v>
       </c>
       <c r="R37" s="14"/>
       <c r="S37" s="15"/>
@@ -1398,7 +1427,7 @@
       <c r="C38" s="5"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q36:Q45" si="0">C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
         <v>0</v>
       </c>
       <c r="R38" s="14"/>
@@ -1419,7 +1448,10 @@
       <c r="B40" s="18"/>
       <c r="C40" s="5"/>
       <c r="P40" s="9"/>
-      <c r="Q40" s="11"/>
+      <c r="Q40" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R40" s="14"/>
       <c r="S40" s="15"/>
     </row>
@@ -1427,7 +1459,10 @@
       <c r="B41" s="18"/>
       <c r="C41" s="5"/>
       <c r="P41" s="9"/>
-      <c r="Q41" s="11"/>
+      <c r="Q41" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R41" s="14"/>
       <c r="S41" s="15"/>
     </row>
@@ -1435,7 +1470,10 @@
       <c r="B42" s="18"/>
       <c r="C42" s="5"/>
       <c r="P42" s="9"/>
-      <c r="Q42" s="11"/>
+      <c r="Q42" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R42" s="14"/>
       <c r="S42" s="15"/>
     </row>
@@ -1443,7 +1481,10 @@
       <c r="B43" s="18"/>
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
-      <c r="Q43" s="11"/>
+      <c r="Q43" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R43" s="14"/>
       <c r="S43" s="15"/>
     </row>
@@ -1451,7 +1492,10 @@
       <c r="B44" s="18"/>
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
-      <c r="Q44" s="11"/>
+      <c r="Q44" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R44" s="14"/>
       <c r="S44" s="15"/>
     </row>
@@ -1471,7 +1515,10 @@
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
       <c r="P45" s="10"/>
-      <c r="Q45" s="11"/>
+      <c r="Q45" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="R45" s="16"/>
       <c r="S45" s="17"/>
     </row>
@@ -1479,8 +1526,8 @@
       <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S35">
-    <sortCondition ref="B35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S37">
+    <sortCondition ref="B37"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q45">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
laborator 26.10.2023 - drum (sau ciclu) hamiltonian prin State
</commit_message>
<xml_diff>
--- a/MatodeAvansate/Prezenta.xlsx
+++ b/MatodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MatodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2157508E-6ED6-4AB8-B504-E95F148788BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B35063-3E21-4937-AE8D-798E6C81EC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -785,7 +785,9 @@
         <v>1</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -797,8 +799,8 @@
       <c r="O3" s="4"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q37" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>1</v>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>2</v>
       </c>
       <c r="R3" s="12"/>
       <c r="S3" s="13"/>
@@ -813,7 +815,7 @@
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="11">
-        <f t="shared" si="0"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
         <v>1</v>
       </c>
       <c r="R4" s="14"/>
@@ -829,7 +831,7 @@
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="11">
-        <f t="shared" si="0"/>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
         <v>1</v>
       </c>
       <c r="R5" s="14"/>
@@ -851,7 +853,7 @@
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="11">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>3</v>
       </c>
       <c r="R6" s="14"/>
@@ -865,10 +867,13 @@
       <c r="E7" t="b">
         <v>1</v>
       </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <v>2</v>
       </c>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
@@ -889,7 +894,7 @@
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="11">
-        <f t="shared" si="0"/>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
         <v>3</v>
       </c>
       <c r="R8" s="14"/>
@@ -907,7 +912,7 @@
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="11">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>2</v>
       </c>
       <c r="R9" s="14"/>
@@ -922,7 +927,7 @@
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="11">
-        <f t="shared" si="0"/>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
         <v>1</v>
       </c>
       <c r="R10" s="14"/>
@@ -941,10 +946,13 @@
       <c r="E11" t="b">
         <v>1</v>
       </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <v>4</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
@@ -967,7 +975,7 @@
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="11">
-        <f t="shared" si="0"/>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
         <v>4</v>
       </c>
       <c r="R12" s="14"/>
@@ -991,7 +999,7 @@
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="11">
-        <f t="shared" si="0"/>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
         <v>4</v>
       </c>
       <c r="R13" s="14"/>
@@ -1015,7 +1023,7 @@
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="11">
-        <f t="shared" si="0"/>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
         <v>4</v>
       </c>
       <c r="R14" s="14"/>
@@ -1036,7 +1044,7 @@
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="11">
-        <f t="shared" si="0"/>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
         <v>3</v>
       </c>
       <c r="R15" s="14"/>
@@ -1044,33 +1052,30 @@
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C16" s="5"/>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>1</v>
       </c>
       <c r="R16" s="14"/>
       <c r="S16" s="15"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
       <c r="E17" t="b">
         <v>1</v>
       </c>
@@ -1079,22 +1084,17 @@
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>4</v>
       </c>
       <c r="R17" s="14"/>
       <c r="S17" s="15"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="E18" t="b">
         <v>1</v>
       </c>
@@ -1103,90 +1103,93 @@
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>2</v>
       </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="C19" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>4</v>
       </c>
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>1</v>
       </c>
       <c r="R20" s="14"/>
       <c r="S20" s="15"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>3</v>
       </c>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>1</v>
       </c>
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C23" s="5"/>
       <c r="D23" t="b">
         <v>1</v>
       </c>
@@ -1198,38 +1201,41 @@
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>3</v>
       </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C24" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <v>4</v>
       </c>
       <c r="R24" s="14"/>
       <c r="S24" s="15"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" t="b">
         <v>1</v>
       </c>
@@ -1238,31 +1244,39 @@
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>2</v>
       </c>
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C26" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>4</v>
       </c>
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" t="b">
@@ -1270,7 +1284,7 @@
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="11">
-        <f t="shared" si="0"/>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
         <v>1</v>
       </c>
       <c r="R27" s="14"/>
@@ -1278,33 +1292,25 @@
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="b">
+        <v>36</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>1</v>
       </c>
       <c r="R28" s="14"/>
       <c r="S28" s="15"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="18" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C29" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="b">
         <v>1</v>
       </c>
       <c r="E29" t="b">
@@ -1315,15 +1321,15 @@
       </c>
       <c r="P29" s="9"/>
       <c r="Q29" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>3</v>
       </c>
       <c r="R29" s="14"/>
       <c r="S29" s="15"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -1339,7 +1345,7 @@
       </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="11">
-        <f t="shared" si="0"/>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
         <v>4</v>
       </c>
       <c r="R30" s="14"/>
@@ -1347,30 +1353,38 @@
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>4</v>
       </c>
       <c r="R31" s="14"/>
       <c r="S31" s="15"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="E32" t="b">
+        <v>25</v>
+      </c>
+      <c r="C32" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="11">
-        <f t="shared" si="0"/>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
         <v>1</v>
       </c>
       <c r="R32" s="14"/>
@@ -1378,63 +1392,66 @@
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D33" t="b">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C33" s="5"/>
       <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="b">
         <v>1</v>
       </c>
       <c r="P33" s="9"/>
       <c r="Q33" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>2</v>
       </c>
       <c r="R33" s="14"/>
       <c r="S33" s="15"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C34" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
       <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>4</v>
       </c>
       <c r="R34" s="14"/>
       <c r="S34" s="15"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
       <c r="E35" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>1</v>
       </c>
       <c r="R35" s="14"/>
       <c r="S35" s="15"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" t="b">
@@ -1445,7 +1462,7 @@
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="11">
-        <f t="shared" si="0"/>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
         <v>2</v>
       </c>
       <c r="R36" s="14"/>
@@ -1453,9 +1470,12 @@
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="18" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C37" s="5"/>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
       <c r="E37" t="b">
         <v>1</v>
       </c>
@@ -1464,8 +1484,8 @@
       </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>3</v>
       </c>
       <c r="R37" s="14"/>
       <c r="S37" s="15"/>
@@ -1480,7 +1500,7 @@
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="11">
-        <f t="shared" ref="Q38:Q45" si="1">C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
         <v>1</v>
       </c>
       <c r="R38" s="14"/>
@@ -1488,16 +1508,19 @@
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C39" s="5"/>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
       <c r="F39" t="b">
         <v>1</v>
       </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>2</v>
       </c>
       <c r="R39" s="14"/>
       <c r="S39" s="15"/>
@@ -1507,7 +1530,7 @@
       <c r="C40" s="5"/>
       <c r="P40" s="9"/>
       <c r="Q40" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q38:Q45" si="0">C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
         <v>0</v>
       </c>
       <c r="R40" s="14"/>
@@ -1518,7 +1541,7 @@
       <c r="C41" s="5"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R41" s="14"/>
@@ -1529,7 +1552,7 @@
       <c r="C42" s="5"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R42" s="14"/>
@@ -1540,7 +1563,7 @@
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R43" s="14"/>
@@ -1551,7 +1574,7 @@
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R44" s="14"/>
@@ -1574,7 +1597,7 @@
       <c r="O45" s="7"/>
       <c r="P45" s="10"/>
       <c r="Q45" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R45" s="16"/>
@@ -1584,8 +1607,8 @@
       <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S37">
-    <sortCondition ref="B37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S39">
+    <sortCondition ref="B39"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q45">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
baza unui algoritm genetic cu solutie simpla si functie de adaptare (fitness) simpla
</commit_message>
<xml_diff>
--- a/MatodeAvansate/Prezenta.xlsx
+++ b/MatodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MatodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFA2818-EA1C-430A-93A0-924C7AE1CB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEF16FF-F6ED-4D5C-BCD2-F1670A2C7C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Lucuta Stefan</t>
+  </si>
+  <si>
+    <t>Tirtea Gabriel</t>
+  </si>
+  <si>
+    <t>Bumb Tudor</t>
   </si>
 </sst>
 </file>
@@ -710,7 +716,7 @@
   <dimension ref="B2:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -799,7 +805,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q39" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>2</v>
       </c>
       <c r="R3" s="12"/>
@@ -815,7 +821,7 @@
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="11">
-        <f t="shared" si="0"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
         <v>1</v>
       </c>
       <c r="R4" s="14"/>
@@ -831,7 +837,7 @@
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="11">
-        <f t="shared" si="0"/>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
         <v>1</v>
       </c>
       <c r="R5" s="14"/>
@@ -856,7 +862,7 @@
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="11">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>4</v>
       </c>
       <c r="R6" s="14"/>
@@ -864,31 +870,25 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="18" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="b">
+      <c r="G7" t="b">
         <v>1</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <v>1</v>
       </c>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="18" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
@@ -900,72 +900,73 @@
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <v>3</v>
       </c>
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="5" t="b">
+        <v>39</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
         <v>1</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <v>4</v>
       </c>
       <c r="R9" s="14"/>
       <c r="S9" s="15"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="18" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <v>2</v>
       </c>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <v>1</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -977,19 +978,22 @@
         <v>1</v>
       </c>
       <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>5</v>
       </c>
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -1005,7 +1009,7 @@
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="11">
-        <f t="shared" si="0"/>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
         <v>4</v>
       </c>
       <c r="R13" s="14"/>
@@ -1013,7 +1017,7 @@
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -1032,7 +1036,7 @@
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="11">
-        <f t="shared" si="0"/>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
         <v>5</v>
       </c>
       <c r="R14" s="14"/>
@@ -1040,9 +1044,12 @@
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="18" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" t="b">
@@ -1056,176 +1063,182 @@
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <v>5</v>
       </c>
       <c r="R15" s="14"/>
       <c r="S15" s="15"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="C16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
       <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>4</v>
       </c>
       <c r="R16" s="14"/>
       <c r="S16" s="15"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C17" s="5"/>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>1</v>
       </c>
       <c r="R17" s="14"/>
       <c r="S17" s="15"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
       <c r="E18" t="b">
         <v>1</v>
       </c>
       <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>5</v>
       </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C19" s="5"/>
       <c r="E19" t="b">
         <v>1</v>
       </c>
       <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>3</v>
       </c>
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="C20" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>4</v>
       </c>
       <c r="R20" s="14"/>
       <c r="S20" s="15"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C21" s="5"/>
       <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>1</v>
       </c>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>3</v>
       </c>
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" t="b">
+        <v>20</v>
+      </c>
+      <c r="C23" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>1</v>
       </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C24" s="5"/>
       <c r="D24" t="b">
         <v>1</v>
       </c>
@@ -1240,74 +1253,91 @@
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <v>4</v>
       </c>
       <c r="R24" s="14"/>
       <c r="S24" s="15"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C25" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D25" t="b">
         <v>1</v>
       </c>
       <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>5</v>
       </c>
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
       </c>
-      <c r="F26" t="b">
+      <c r="G26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>3</v>
       </c>
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C27" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>5</v>
       </c>
       <c r="R27" s="14"/>
       <c r="S27" s="15"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" t="b">
@@ -1315,7 +1345,7 @@
       </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="11">
-        <f t="shared" si="0"/>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
         <v>1</v>
       </c>
       <c r="R28" s="14"/>
@@ -1323,55 +1353,44 @@
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="b">
+        <v>36</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" t="b">
         <v>1</v>
       </c>
       <c r="P29" s="9"/>
       <c r="Q29" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>1</v>
       </c>
       <c r="R29" s="14"/>
       <c r="S29" s="15"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="18" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
       <c r="E30" t="b">
         <v>1</v>
       </c>
       <c r="F30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" t="b">
         <v>1</v>
       </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>3</v>
       </c>
       <c r="R30" s="14"/>
       <c r="S30" s="15"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
@@ -1390,7 +1409,7 @@
       </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="11">
-        <f t="shared" si="0"/>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
         <v>5</v>
       </c>
       <c r="R31" s="14"/>
@@ -1398,9 +1417,18 @@
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="b">
         <v>1</v>
       </c>
       <c r="G32" t="b">
@@ -1408,26 +1436,25 @@
       </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>5</v>
       </c>
       <c r="R32" s="14"/>
       <c r="S32" s="15"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="E33" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" t="b">
+        <v>25</v>
+      </c>
+      <c r="C33" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
         <v>1</v>
       </c>
       <c r="P33" s="9"/>
       <c r="Q33" s="11">
-        <f t="shared" si="0"/>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
         <v>2</v>
       </c>
       <c r="R33" s="14"/>
@@ -1435,14 +1462,9 @@
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D34" t="b">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C34" s="5"/>
       <c r="E34" t="b">
         <v>1</v>
       </c>
@@ -1454,53 +1476,58 @@
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>3</v>
       </c>
       <c r="R34" s="14"/>
       <c r="S34" s="15"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C35" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
       <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" t="b">
         <v>1</v>
       </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>5</v>
       </c>
       <c r="R35" s="14"/>
       <c r="S35" s="15"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
       <c r="E36" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" t="b">
         <v>1</v>
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <v>1</v>
       </c>
       <c r="R36" s="14"/>
       <c r="S36" s="15"/>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" t="b">
@@ -1509,12 +1536,12 @@
       <c r="E37" t="b">
         <v>1</v>
       </c>
-      <c r="F37" t="b">
+      <c r="G37" t="b">
         <v>1</v>
       </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="11">
-        <f t="shared" si="0"/>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
         <v>3</v>
       </c>
       <c r="R37" s="14"/>
@@ -1522,15 +1549,15 @@
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="F38" t="b">
+      <c r="G38" t="b">
         <v>1</v>
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="11">
-        <f t="shared" si="0"/>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
         <v>1</v>
       </c>
       <c r="R38" s="14"/>
@@ -1538,9 +1565,12 @@
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="18" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C39" s="5"/>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
       <c r="E39" t="b">
         <v>1</v>
       </c>
@@ -1552,30 +1582,49 @@
       </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>4</v>
       </c>
       <c r="R39" s="14"/>
       <c r="S39" s="15"/>
     </row>
     <row r="40" spans="2:19">
-      <c r="B40" s="18"/>
+      <c r="B40" s="18" t="s">
+        <v>53</v>
+      </c>
       <c r="C40" s="5"/>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
       <c r="P40" s="9"/>
       <c r="Q40" s="11">
-        <f t="shared" ref="Q40:Q45" si="1">C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
-        <v>0</v>
+        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <v>2</v>
       </c>
       <c r="R40" s="14"/>
       <c r="S40" s="15"/>
     </row>
     <row r="41" spans="2:19">
-      <c r="B41" s="18"/>
+      <c r="B41" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="C41" s="5"/>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <v>3</v>
       </c>
       <c r="R41" s="14"/>
       <c r="S41" s="15"/>
@@ -1585,7 +1634,7 @@
       <c r="C42" s="5"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q40:Q45" si="0">C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
         <v>0</v>
       </c>
       <c r="R42" s="14"/>
@@ -1596,7 +1645,7 @@
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R43" s="14"/>
@@ -1607,7 +1656,7 @@
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R44" s="14"/>
@@ -1630,7 +1679,7 @@
       <c r="O45" s="7"/>
       <c r="P45" s="10"/>
       <c r="Q45" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R45" s="16"/>
@@ -1640,8 +1689,8 @@
       <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S39">
-    <sortCondition ref="B39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S41">
+    <sortCondition ref="B3:B41"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q45">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
added articlePage, userPage, bootstrap icons, userService
</commit_message>
<xml_diff>
--- a/MatodeAvansate/Prezenta.xlsx
+++ b/MatodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MatodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEF16FF-F6ED-4D5C-BCD2-F1670A2C7C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7A9D4A-AE27-4901-BFB8-457081637A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Bumb Tudor</t>
+  </si>
+  <si>
+    <t>Cozariuc Vicentiu</t>
   </si>
 </sst>
 </file>
@@ -716,7 +719,7 @@
   <dimension ref="B2:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A42" sqref="A3:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -860,10 +863,13 @@
       <c r="G6" t="b">
         <v>1</v>
       </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="11">
         <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R6" s="14"/>
       <c r="S6" s="15"/>
@@ -908,92 +914,84 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="18" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" t="b">
+      <c r="H9" t="b">
         <v>1</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="11">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R9" s="14"/>
       <c r="S9" s="15"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="5" t="b">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="11">
         <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="18" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="11">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="11">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -1005,19 +1003,22 @@
         <v>1</v>
       </c>
       <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="11">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -1029,22 +1030,19 @@
         <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="11">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -1059,23 +1057,29 @@
         <v>1</v>
       </c>
       <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="11">
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R15" s="14"/>
       <c r="S15" s="15"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="18" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
       <c r="E16" t="b">
         <v>1</v>
       </c>
@@ -1083,64 +1087,72 @@
         <v>1</v>
       </c>
       <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="11">
         <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R16" s="14"/>
       <c r="S16" s="15"/>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="C17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
       <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="11">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R17" s="14"/>
       <c r="S17" s="15"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="11">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
       <c r="E19" t="b">
         <v>1</v>
       </c>
@@ -1148,124 +1160,125 @@
         <v>1</v>
       </c>
       <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="11">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="E20" t="b">
         <v>1</v>
       </c>
       <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="11">
         <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R20" s="14"/>
       <c r="S20" s="15"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="C21" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="11">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="11">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" t="b">
         <v>1</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="11">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" t="b">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="11">
         <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R24" s="14"/>
       <c r="S24" s="15"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" t="b">
         <v>1</v>
       </c>
@@ -1281,47 +1294,50 @@
       <c r="P25" s="9"/>
       <c r="Q25" s="11">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C26" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
       </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
       <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="11">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C27" s="5"/>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="G27" t="b">
@@ -1330,30 +1346,41 @@
       <c r="P27" s="9"/>
       <c r="Q27" s="11">
         <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R27" s="14"/>
       <c r="S27" s="15"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C28" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
         <v>1</v>
       </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="11">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R28" s="14"/>
       <c r="S28" s="15"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" t="b">
@@ -1369,55 +1396,44 @@
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" t="b">
+        <v>36</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" t="b">
         <v>1</v>
       </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="11">
         <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R30" s="14"/>
       <c r="S30" s="15"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="18" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C31" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
       <c r="E31" t="b">
         <v>1</v>
       </c>
       <c r="F31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" t="b">
         <v>1</v>
       </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="11">
         <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R31" s="14"/>
       <c r="S31" s="15"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="5" t="b">
         <v>1</v>
@@ -1432,43 +1448,54 @@
         <v>1</v>
       </c>
       <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="11">
         <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R32" s="14"/>
       <c r="S32" s="15"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
       <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
         <v>1</v>
       </c>
       <c r="P33" s="9"/>
       <c r="Q33" s="11">
         <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R33" s="14"/>
       <c r="S33" s="15"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="b">
+        <v>25</v>
+      </c>
+      <c r="C34" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G34" t="b">
@@ -1477,21 +1504,16 @@
       <c r="P34" s="9"/>
       <c r="Q34" s="11">
         <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R34" s="14"/>
       <c r="S34" s="15"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C35" s="5"/>
       <c r="E35" t="b">
         <v>1</v>
       </c>
@@ -1504,95 +1526,109 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="11">
         <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R35" s="14"/>
       <c r="S35" s="15"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C36" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
       <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
         <v>1</v>
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="11">
         <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R36" s="14"/>
       <c r="S36" s="15"/>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
       <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" t="b">
         <v>1</v>
       </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="11">
         <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R37" s="14"/>
       <c r="S37" s="15"/>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="18" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C38" s="5"/>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
       <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
         <v>1</v>
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="11">
         <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R38" s="14"/>
       <c r="S38" s="15"/>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="18" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
       <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
         <v>1</v>
       </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="11">
         <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R39" s="14"/>
       <c r="S39" s="15"/>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="18" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C40" s="5"/>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
       <c r="F40" t="b">
         <v>1</v>
       </c>
@@ -1602,19 +1638,16 @@
       <c r="P40" s="9"/>
       <c r="Q40" s="11">
         <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R40" s="14"/>
       <c r="S40" s="15"/>
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="E41" t="b">
-        <v>1</v>
-      </c>
       <c r="F41" t="b">
         <v>1</v>
       </c>
@@ -1624,18 +1657,32 @@
       <c r="P41" s="9"/>
       <c r="Q41" s="11">
         <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R41" s="14"/>
       <c r="S41" s="15"/>
     </row>
     <row r="42" spans="2:19">
-      <c r="B42" s="18"/>
+      <c r="B42" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="C42" s="5"/>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="9"/>
       <c r="Q42" s="11">
-        <f t="shared" ref="Q40:Q45" si="0">C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
-        <v>0</v>
+        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <v>4</v>
       </c>
       <c r="R42" s="14"/>
       <c r="S42" s="15"/>
@@ -1645,7 +1692,7 @@
       <c r="C43" s="5"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q42:Q45" si="0">C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
         <v>0</v>
       </c>
       <c r="R43" s="14"/>
@@ -1689,8 +1736,8 @@
       <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S41">
-    <sortCondition ref="B3:B41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S42">
+    <sortCondition ref="B42"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q45">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 09.11.2023: Liste create de utilizator si parcurgerile in graf
</commit_message>
<xml_diff>
--- a/MatodeAvansate/Prezenta.xlsx
+++ b/MatodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MatodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7A9D4A-AE27-4901-BFB8-457081637A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1043C6-29B0-4054-AC84-402191C5639D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Cozariuc Vicentiu</t>
+  </si>
+  <si>
+    <t>Pintilie Robert</t>
   </si>
 </sst>
 </file>
@@ -718,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A42" sqref="A3:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -882,10 +885,13 @@
       <c r="G7" t="b">
         <v>1</v>
       </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="11">
         <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
@@ -904,10 +910,13 @@
       <c r="G8" t="b">
         <v>1</v>
       </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="11">
         <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
@@ -1008,10 +1017,13 @@
       <c r="G13" t="b">
         <v>1</v>
       </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="11">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
@@ -1032,10 +1044,13 @@
       <c r="F14" t="b">
         <v>1</v>
       </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="11">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
@@ -1291,10 +1306,13 @@
       <c r="G25" t="b">
         <v>1</v>
       </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="11">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R25" s="14"/>
       <c r="S25" s="15"/>
@@ -1343,10 +1361,13 @@
       <c r="G27" t="b">
         <v>1</v>
       </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="11">
         <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R27" s="14"/>
       <c r="S27" s="15"/>
@@ -1370,10 +1391,13 @@
       <c r="G28" t="b">
         <v>1</v>
       </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="11">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R28" s="14"/>
       <c r="S28" s="15"/>
@@ -1386,10 +1410,13 @@
       <c r="D29" t="b">
         <v>1</v>
       </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="9"/>
       <c r="Q29" s="11">
         <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R29" s="14"/>
       <c r="S29" s="15"/>
@@ -1433,37 +1460,23 @@
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" t="b">
-        <v>1</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C32" s="5"/>
       <c r="H32" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="11">
         <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="R32" s="14"/>
       <c r="S32" s="15"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="5" t="b">
         <v>1</v>
@@ -1493,31 +1506,39 @@
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
       <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
         <v>1</v>
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="11">
         <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R34" s="14"/>
       <c r="S34" s="15"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="b">
+        <v>25</v>
+      </c>
+      <c r="C35" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G35" t="b">
@@ -1526,21 +1547,16 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="11">
         <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R35" s="14"/>
       <c r="S35" s="15"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C36" s="5"/>
       <c r="E36" t="b">
         <v>1</v>
       </c>
@@ -1553,57 +1569,65 @@
       <c r="P36" s="9"/>
       <c r="Q36" s="11">
         <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R36" s="14"/>
       <c r="S36" s="15"/>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C37" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
       <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
         <v>1</v>
       </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="11">
         <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R37" s="14"/>
       <c r="S37" s="15"/>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" t="b">
-        <v>1</v>
-      </c>
       <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" t="b">
         <v>1</v>
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="11">
         <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R38" s="14"/>
       <c r="S38" s="15"/>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="18" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C39" s="5"/>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
       <c r="G39" t="b">
         <v>1</v>
       </c>
@@ -1613,87 +1637,98 @@
       <c r="P39" s="9"/>
       <c r="Q39" s="11">
         <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R39" s="14"/>
       <c r="S39" s="15"/>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="18" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" t="b">
-        <v>1</v>
-      </c>
       <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
         <v>1</v>
       </c>
       <c r="P40" s="9"/>
       <c r="Q40" s="11">
         <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R40" s="14"/>
       <c r="S40" s="15"/>
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="18" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C41" s="5"/>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
       <c r="F41" t="b">
         <v>1</v>
       </c>
       <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
         <v>1</v>
       </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="11">
         <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R41" s="14"/>
       <c r="S41" s="15"/>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="E42" t="b">
-        <v>1</v>
-      </c>
       <c r="F42" t="b">
         <v>1</v>
       </c>
       <c r="G42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" t="b">
         <v>1</v>
       </c>
       <c r="P42" s="9"/>
       <c r="Q42" s="11">
         <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R42" s="14"/>
       <c r="S42" s="15"/>
     </row>
     <row r="43" spans="2:19">
-      <c r="B43" s="18"/>
+      <c r="B43" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="C43" s="5"/>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
       <c r="P43" s="9"/>
       <c r="Q43" s="11">
-        <f t="shared" ref="Q42:Q45" si="0">C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
-        <v>0</v>
+        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
+        <v>4</v>
       </c>
       <c r="R43" s="14"/>
       <c r="S43" s="15"/>
@@ -1703,7 +1738,7 @@
       <c r="C44" s="5"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q43:Q45" si="0">C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
         <v>0</v>
       </c>
       <c r="R44" s="14"/>
@@ -1736,8 +1771,8 @@
       <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S42">
-    <sortCondition ref="B42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S43">
+    <sortCondition ref="B43"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q45">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>